<commit_message>
prism now works for wes
</commit_message>
<xml_diff>
--- a/template_examples/wes_template.xlsx
+++ b/template_examples/wes_template.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27715"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27417"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/md299/PycharmProjects/cidc-schemas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlindsay/Documents/Code/cidc/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="35360" windowHeight="16360"/>
+    <workbookView xWindow="-38620" yWindow="5740" windowWidth="35360" windowHeight="16360"/>
   </bookViews>
   <sheets>
     <sheet name="WES" sheetId="1" r:id="rId1"/>
@@ -171,7 +171,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>The type of material submitted - tumor/normal/etc</t>
+          <t>Aliquot identifier assigned by the CIMAC-CIDC Network. Example: CIMAC-12453.</t>
         </r>
       </text>
     </comment>
@@ -184,7 +184,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Lot number for the library construction kit</t>
+          <t>The type of material submitted - tumor/normal/etc</t>
         </r>
       </text>
     </comment>
@@ -197,7 +197,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Lot number for the bait set</t>
+          <t>Lot number for the library construction kit</t>
         </r>
       </text>
     </comment>
@@ -210,7 +210,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Date of library construction.</t>
+          <t>Lot number for the bait set</t>
         </r>
       </text>
     </comment>
@@ -223,7 +223,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Date of the hybrid capture enrichment</t>
+          <t>Date of library construction.</t>
         </r>
       </text>
     </comment>
@@ -236,7 +236,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Amount of DNA/RNA (in ng) used for library construction</t>
+          <t>Date of the hybrid capture enrichment</t>
         </r>
       </text>
     </comment>
@@ -249,7 +249,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Resulting yield (in ng) from library construction</t>
+          <t>Amount of DNA/RNA (in ng) used for library construction</t>
         </r>
       </text>
     </comment>
@@ -262,7 +262,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>The average insert size for the library</t>
+          <t>Resulting yield (in ng) from library construction</t>
         </r>
       </text>
     </comment>
@@ -275,7 +275,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Path to a file on a users computer</t>
+          <t>The average insert size for the library</t>
         </r>
       </text>
     </comment>
@@ -305,12 +305,25 @@
         </r>
       </text>
     </comment>
+    <comment ref="O12" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Path to a file on a users computer</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="45">
   <si>
     <t>#t</t>
   </si>
@@ -405,9 +418,6 @@
     <t>KAPA - Hyper Prep</t>
   </si>
   <si>
-    <t>Illumina - HiSeq 3000</t>
-  </si>
-  <si>
     <t>Paired</t>
   </si>
   <si>
@@ -439,6 +449,15 @@
   </si>
   <si>
     <t>gs://path/to/read_group_map.txt</t>
+  </si>
+  <si>
+    <t>Illumina - NextSeq 550</t>
+  </si>
+  <si>
+    <t>CIMAC SAMPLE ID</t>
+  </si>
+  <si>
+    <t>sample 1</t>
   </si>
 </sst>
 </file>
@@ -540,10 +559,10 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -845,10 +864,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N212"/>
+  <dimension ref="A1:O212"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -857,27 +876,27 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -899,7 +918,7 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -921,7 +940,7 @@
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -943,7 +962,7 @@
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -965,7 +984,7 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -987,7 +1006,7 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -995,7 +1014,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -1009,7 +1028,7 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -1017,7 +1036,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1031,7 +1050,7 @@
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -1053,24 +1072,24 @@
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B11" s="3" t="s">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1078,136 +1097,145 @@
         <v>14</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="I12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="J12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="K12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="L12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="L12" s="2" t="s">
+      <c r="M12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="M12" s="2" t="s">
+      <c r="N12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="N12" s="2" t="s">
+      <c r="O12" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" t="s">
         <v>33</v>
       </c>
-      <c r="C13" t="s">
+      <c r="E13" t="s">
         <v>34</v>
       </c>
-      <c r="D13" t="s">
+      <c r="F13" t="s">
         <v>35</v>
       </c>
-      <c r="E13" t="s">
+      <c r="G13" t="s">
         <v>36</v>
       </c>
-      <c r="F13" t="s">
+      <c r="H13" s="3">
+        <v>43586</v>
+      </c>
+      <c r="I13" s="3">
+        <v>43587</v>
+      </c>
+      <c r="J13">
+        <v>100</v>
+      </c>
+      <c r="K13">
+        <v>700</v>
+      </c>
+      <c r="L13">
+        <v>250</v>
+      </c>
+      <c r="M13" t="s">
+        <v>39</v>
+      </c>
+      <c r="N13" t="s">
+        <v>40</v>
+      </c>
+      <c r="O13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" t="s">
         <v>37</v>
       </c>
-      <c r="G13" s="4">
+      <c r="E14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" t="s">
+        <v>36</v>
+      </c>
+      <c r="H14" s="3">
         <v>43586</v>
       </c>
-      <c r="H13" s="4">
+      <c r="I14" s="3">
         <v>43587</v>
       </c>
-      <c r="I13">
+      <c r="J14">
         <v>100</v>
       </c>
-      <c r="J13">
+      <c r="K14">
         <v>700</v>
       </c>
-      <c r="K13">
+      <c r="L14">
         <v>250</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M14" t="s">
+        <v>39</v>
+      </c>
+      <c r="N14" t="s">
         <v>40</v>
       </c>
-      <c r="M13" t="s">
+      <c r="O14" t="s">
         <v>41</v>
       </c>
-      <c r="N13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" t="s">
-        <v>36</v>
-      </c>
-      <c r="F14" t="s">
-        <v>37</v>
-      </c>
-      <c r="G14" s="4">
-        <v>43586</v>
-      </c>
-      <c r="H14" s="4">
-        <v>43587</v>
-      </c>
-      <c r="I14">
-        <v>100</v>
-      </c>
-      <c r="J14">
-        <v>700</v>
-      </c>
-      <c r="K14">
-        <v>250</v>
-      </c>
-      <c r="L14" t="s">
-        <v>40</v>
-      </c>
-      <c r="M14" t="s">
-        <v>41</v>
-      </c>
-      <c r="N14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -2216,14 +2244,14 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8">
       <formula1>"Paired,Single"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D13:D212">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="G15:H212">
+      <formula1>AND(ISNUMBER(G15:G214),LEFT(CELL("format",G15:G214),1)="D")</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D15:D212 E13:E14">
       <formula1>"Tumor,Normal,Metastasis"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="G15:G212 G13:H14">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="H13:I14">
       <formula1>AND(ISNUMBER(G13:G212),LEFT(CELL("format",G13:G212),1)="D")</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="H15:H212">
-      <formula1>AND(ISNUMBER(H15:H214),LEFT(CELL("format",H15:H214),1)="D")</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Prism rework for json pointers instead of grep and hints
</commit_message>
<xml_diff>
--- a/template_examples/wes_template.xlsx
+++ b/template_examples/wes_template.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C12A165-F286-CF4B-9BA1-01B636490A57}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67FFEE78-5216-A14C-84BD-357B051D5608}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8860" yWindow="6800" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15720" yWindow="4140" windowWidth="33920" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WES" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -90,7 +91,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -142,7 +143,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -150,12 +151,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="D11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
+    <comment ref="D11" authorId="0" shapeId="0" xr:uid="{CCABD995-AC02-4245-ABB7-232AF179A1F6}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -163,20 +164,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>The type of material submitted - tumor/normal/etc</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
+    <comment ref="E11" authorId="0" shapeId="0" xr:uid="{5FD44912-A6D4-F047-A8D4-0929F5160171}">
       <text>
         <r>
           <rPr>
@@ -189,7 +177,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
+    <comment ref="F11" authorId="0" shapeId="0" xr:uid="{BD591F88-7A6E-624F-A21F-0A9BE82F061D}">
       <text>
         <r>
           <rPr>
@@ -202,7 +190,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
+    <comment ref="G11" authorId="0" shapeId="0" xr:uid="{72B04301-8BD6-1D4A-B870-8E64C017BB50}">
       <text>
         <r>
           <rPr>
@@ -215,7 +203,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
+    <comment ref="H11" authorId="0" shapeId="0" xr:uid="{597DD51F-1054-5348-9539-56357F47D06F}">
       <text>
         <r>
           <rPr>
@@ -228,7 +216,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
+    <comment ref="I11" authorId="0" shapeId="0" xr:uid="{E5FB80EC-0A0B-CB46-9FD1-C96C1F1C0D25}">
       <text>
         <r>
           <rPr>
@@ -241,7 +229,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
+    <comment ref="J11" authorId="0" shapeId="0" xr:uid="{4ECCEB21-8832-F845-B56A-8923A3F147F8}">
       <text>
         <r>
           <rPr>
@@ -254,7 +242,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
+    <comment ref="K11" authorId="0" shapeId="0" xr:uid="{8C6BF389-6DE0-E145-8A81-272A506F4F18}">
       <text>
         <r>
           <rPr>
@@ -267,7 +255,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="M11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
+    <comment ref="L11" authorId="0" shapeId="0" xr:uid="{03E96CD9-7FE0-CA42-A5AF-E1F09FC130FB}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Path to a file on a users computer</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M11" authorId="0" shapeId="0" xr:uid="{91700150-A7BA-BB43-8D20-7415C3F9727B}">
       <text>
         <r>
           <rPr>
@@ -280,20 +281,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Path to a file on a users computer</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="O11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
+    <comment ref="N11" authorId="0" shapeId="0" xr:uid="{45C40F77-8854-5048-B133-FD6640EB5749}">
       <text>
         <r>
           <rPr>
@@ -311,7 +299,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="42">
   <si>
     <t>#t</t>
   </si>
@@ -358,9 +346,6 @@
     <t>CIMAC ALIQUOT ID</t>
   </si>
   <si>
-    <t>GENOMIC SOURCE</t>
-  </si>
-  <si>
     <t>LIBRARY KIT LOT</t>
   </si>
   <si>
@@ -403,27 +388,12 @@
     <t>Paired</t>
   </si>
   <si>
-    <t>Patient 1</t>
-  </si>
-  <si>
-    <t>aliquot 1</t>
-  </si>
-  <si>
-    <t>Tumor</t>
-  </si>
-  <si>
     <t>lot abc</t>
   </si>
   <si>
     <t>lot 123</t>
   </si>
   <si>
-    <t>aliquot 2</t>
-  </si>
-  <si>
-    <t>Normal</t>
-  </si>
-  <si>
     <t>gs://path/to/fwd.fastq</t>
   </si>
   <si>
@@ -439,7 +409,22 @@
     <t>CIMAC SAMPLE ID</t>
   </si>
   <si>
-    <t>sample 1</t>
+    <t>wes example PA 1</t>
+  </si>
+  <si>
+    <t>wes example PA 2</t>
+  </si>
+  <si>
+    <t>wes example SA 1.1</t>
+  </si>
+  <si>
+    <t>wes example SA 2.1</t>
+  </si>
+  <si>
+    <t>wes example aliquot 1.1.1</t>
+  </si>
+  <si>
+    <t>wes example aliquot 1.2.1</t>
   </si>
 </sst>
 </file>
@@ -855,19 +840,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O211"/>
+  <dimension ref="A1:N211"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B4" sqref="A4:XFD4"/>
+      <selection activeCell="E2" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
-    <col min="2" max="101" width="30.6640625" customWidth="1"/>
+    <col min="2" max="95" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -880,14 +865,8 @@
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-    </row>
-    <row r="2" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -902,14 +881,8 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-    </row>
-    <row r="3" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -917,21 +890,15 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-    </row>
-    <row r="4" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -939,21 +906,15 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-    </row>
-    <row r="5" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -961,21 +922,15 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-    </row>
-    <row r="6" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -983,21 +938,15 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-    </row>
-    <row r="7" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1005,21 +954,15 @@
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-    </row>
-    <row r="8" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -1034,14 +977,8 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
@@ -1051,14 +988,8 @@
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1066,7 +997,7 @@
         <v>13</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>14</v>
@@ -1101,1100 +1032,1091 @@
       <c r="N11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="O11" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" t="s">
         <v>30</v>
       </c>
-      <c r="C12" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="G12" s="3">
+        <v>43586</v>
+      </c>
+      <c r="H12" s="3">
+        <v>43587</v>
+      </c>
+      <c r="I12">
+        <v>100</v>
+      </c>
+      <c r="J12">
+        <v>700</v>
+      </c>
+      <c r="K12">
+        <v>250</v>
+      </c>
+      <c r="L12" t="s">
         <v>31</v>
       </c>
-      <c r="E12" t="s">
+      <c r="M12" t="s">
         <v>32</v>
       </c>
-      <c r="F12" t="s">
+      <c r="N12" t="s">
         <v>33</v>
       </c>
-      <c r="G12" t="s">
-        <v>34</v>
-      </c>
-      <c r="H12" s="3">
+    </row>
+    <row r="13" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="3">
         <v>43586</v>
       </c>
-      <c r="I12" s="3">
+      <c r="H13" s="3">
         <v>43587</v>
       </c>
-      <c r="J12">
+      <c r="I13">
         <v>100</v>
       </c>
-      <c r="K12">
+      <c r="J13">
         <v>700</v>
       </c>
-      <c r="L12">
+      <c r="K13">
         <v>250</v>
       </c>
-      <c r="M12" t="s">
-        <v>37</v>
-      </c>
-      <c r="N12" t="s">
-        <v>38</v>
-      </c>
-      <c r="O12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" t="s">
-        <v>36</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="L13" t="s">
+        <v>31</v>
+      </c>
+      <c r="M13" t="s">
+        <v>32</v>
+      </c>
+      <c r="N13" t="s">
         <v>33</v>
       </c>
-      <c r="G13" t="s">
-        <v>34</v>
-      </c>
-      <c r="H13" s="3">
-        <v>43586</v>
-      </c>
-      <c r="I13" s="3">
-        <v>43587</v>
-      </c>
-      <c r="J13">
-        <v>100</v>
-      </c>
-      <c r="K13">
-        <v>700</v>
-      </c>
-      <c r="L13">
-        <v>250</v>
-      </c>
-      <c r="M13" t="s">
-        <v>37</v>
-      </c>
-      <c r="N13" t="s">
-        <v>38</v>
-      </c>
-      <c r="O13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B1:N1"/>
-    <mergeCell ref="B10:N10"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B10:H10"/>
   </mergeCells>
-  <dataValidations count="8">
+  <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"DFCI,Mount Sinai, Stanford, MD Anderson"</formula1>
     </dataValidation>
@@ -2210,14 +2132,8 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"Paired,Single"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="G14:H211" xr:uid="{00000000-0002-0000-0000-000006000000}">
-      <formula1>AND(ISNUMBER(G14:G213),LEFT(CELL("format",G14:G213),1)="D")</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D14:D211 E12:E13" xr:uid="{00000000-0002-0000-0000-000007000000}">
-      <formula1>"Tumor,Normal,Metastasis"</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="H12:I13" xr:uid="{00000000-0002-0000-0000-000008000000}">
-      <formula1>AND(ISNUMBER(G12:G211),LEFT(CELL("format",G12:G211),1)="D")</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="G12:H13" xr:uid="{0E2C5848-830B-E540-BBDC-854F9CE5A3A2}">
+      <formula1>AND(ISNUMBER(E12:E211),LEFT(CELL("format",E12:E211),1)="D")</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
prism for wes embeded in a new way
</commit_message>
<xml_diff>
--- a/template_examples/wes_template.xlsx
+++ b/template_examples/wes_template.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67FFEE78-5216-A14C-84BD-357B051D5608}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEFD973D-1928-7644-B8E2-2056376DAF3C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15720" yWindow="4140" windowWidth="33920" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14520" yWindow="1740" windowWidth="28800" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WES" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -299,7 +298,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="47">
   <si>
     <t>#t</t>
   </si>
@@ -388,21 +387,6 @@
     <t>Paired</t>
   </si>
   <si>
-    <t>lot abc</t>
-  </si>
-  <si>
-    <t>lot 123</t>
-  </si>
-  <si>
-    <t>gs://path/to/fwd.fastq</t>
-  </si>
-  <si>
-    <t>gs://path/to/rev.fastq</t>
-  </si>
-  <si>
-    <t>gs://path/to/read_group_map.txt</t>
-  </si>
-  <si>
     <t>Illumina - NextSeq 550</t>
   </si>
   <si>
@@ -425,6 +409,36 @@
   </si>
   <si>
     <t>wes example aliquot 1.2.1</t>
+  </si>
+  <si>
+    <t>e lot 1.2.1</t>
+  </si>
+  <si>
+    <t>e lot 1.1.1</t>
+  </si>
+  <si>
+    <t>l lot 1.1.1</t>
+  </si>
+  <si>
+    <t>l loc 1.2.1</t>
+  </si>
+  <si>
+    <t>/local/path/to/fwd.1.1.1.fastq</t>
+  </si>
+  <si>
+    <t>/local/path/to/fwd.1.2.1.fastq</t>
+  </si>
+  <si>
+    <t>/local/path/to/rev.1.1.1.fastq</t>
+  </si>
+  <si>
+    <t>/local/path/to/rev.1.2.1.fastq</t>
+  </si>
+  <si>
+    <t>/local/path/to/rgm.1.1.1.txt</t>
+  </si>
+  <si>
+    <t>/local/path/to/rgm.1.2.1.txt</t>
   </si>
 </sst>
 </file>
@@ -843,7 +857,7 @@
   <dimension ref="A1:N211"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E1:E1048576"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -938,7 +952,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -997,7 +1011,7 @@
         <v>13</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>14</v>
@@ -1038,19 +1052,19 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" t="s">
         <v>38</v>
-      </c>
-      <c r="D12" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" t="s">
-        <v>29</v>
-      </c>
-      <c r="F12" t="s">
-        <v>30</v>
       </c>
       <c r="G12" s="3">
         <v>43586</v>
@@ -1059,22 +1073,22 @@
         <v>43587</v>
       </c>
       <c r="I12">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J12">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="K12">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="L12" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="M12" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="N12" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1082,19 +1096,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" t="s">
         <v>37</v>
-      </c>
-      <c r="C13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" t="s">
-        <v>30</v>
       </c>
       <c r="G13" s="3">
         <v>43586</v>
@@ -1103,22 +1117,22 @@
         <v>43587</v>
       </c>
       <c r="I13">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="J13">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="K13">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="L13" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="M13" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="N13" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update wes metadata template
</commit_message>
<xml_diff>
--- a/template_examples/wes_template.xlsx
+++ b/template_examples/wes_template.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7127A892-FC0B-DB4B-AF23-BB7FC78E31F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2003E7DD-E808-D14B-ACE1-0217443741E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7340" yWindow="3560" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7880" yWindow="5000" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WES" sheetId="1" r:id="rId1"/>
+    <sheet name="Legend" sheetId="2" r:id="rId2"/>
+    <sheet name="Data Dictionary" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -82,7 +84,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -212,7 +214,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="71">
   <si>
     <t>#t</t>
   </si>
@@ -232,7 +234,7 @@
     <t>Assay creator</t>
   </si>
   <si>
-    <t>Sequencing_protocol</t>
+    <t>Sequencing protocol</t>
   </si>
   <si>
     <t>Library kit</t>
@@ -268,59 +270,170 @@
     <t>Reverse fastq</t>
   </si>
   <si>
-    <t>Sequencing_date</t>
-  </si>
-  <si>
-    <t>Quality_flag</t>
+    <t>Sequencing date</t>
+  </si>
+  <si>
+    <t>Quality flag</t>
+  </si>
+  <si>
+    <t>LEGEND</t>
+  </si>
+  <si>
+    <t>Legend for tab 'WES'</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>User defined unique identifier for this assay run.</t>
+  </si>
+  <si>
+    <t>Trial identifier used by lead organization, ie. Center for Experimental Therapeutics Program (CTEP) ID or Industry Sponsored ID.  This is usually a short identifier. Example: E4412.</t>
+  </si>
+  <si>
+    <t>Enum</t>
+  </si>
+  <si>
+    <t>Indicates what site is filling out the assay.</t>
+  </si>
+  <si>
+    <t>E.g. 'DFCI'</t>
+  </si>
+  <si>
+    <t>Protocol and version used for the sequencing.</t>
+  </si>
+  <si>
+    <t>E.g. 'Express Somatic Human WES (Deep Coverage) v1.1'</t>
+  </si>
+  <si>
+    <t>The library construction kit.</t>
+  </si>
+  <si>
+    <t>E.g. 'Hyper Prep ICE Exome Express: 1.0'</t>
+  </si>
+  <si>
+    <t>Sequencer Model, e.g. HiSeq 2500, NextSeq, NovaSeq.</t>
+  </si>
+  <si>
+    <t>E.g. 'Illumina - HiSeq 2500'</t>
+  </si>
+  <si>
+    <t>Indicates if the sequencing was performed paired or single ended.</t>
+  </si>
+  <si>
+    <t>E.g. 'Paired'</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>Number of cycles for each sequencing read.</t>
+  </si>
+  <si>
+    <t>Bait set ID.</t>
+  </si>
+  <si>
+    <t>E.g. 'whole_exome_illumina_coding_v1'</t>
+  </si>
+  <si>
+    <t>Section 'Samples' of tab 'WES'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">String: regex ^C[A-Z0-9]{3}[A-Z0-9]{3}[A-Z0-9]{2}.[0-9]{2}$ </t>
+  </si>
+  <si>
+    <t>Specimen identifier assigned by the CIMAC-CIDC Network. Formatted as C????????.??</t>
+  </si>
+  <si>
+    <t>E.g. 'CTTTP01A1.00'</t>
+  </si>
+  <si>
+    <t>Path to a file on a user's computer.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">String: date </t>
+  </si>
+  <si>
+    <t>Date of sequencing.</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Flag used for quality.</t>
+  </si>
+  <si>
+    <t>DFCI</t>
+  </si>
+  <si>
+    <t>Mount Sinai</t>
+  </si>
+  <si>
+    <t>Stanford</t>
+  </si>
+  <si>
+    <t>MD Anderson</t>
+  </si>
+  <si>
+    <t>Express Somatic Human WES (Deep Coverage) v1.1</t>
+  </si>
+  <si>
+    <t>Hyper Prep ICE Exome Express: 1.0</t>
+  </si>
+  <si>
+    <t>Illumina - HiSeq 2500</t>
+  </si>
+  <si>
+    <t>Illumina - HiSeq 3000</t>
+  </si>
+  <si>
+    <t>Illumina - NextSeq 550</t>
+  </si>
+  <si>
+    <t>Illumina - HiSeq 4000</t>
+  </si>
+  <si>
+    <t>Illumina - NovaSeq 6000</t>
+  </si>
+  <si>
+    <t>Paired</t>
+  </si>
+  <si>
+    <t>Single</t>
+  </si>
+  <si>
+    <t>whole_exome_illumina_coding_v1</t>
+  </si>
+  <si>
+    <t>test_prism_trial_id_run_1</t>
   </si>
   <si>
     <t>test_prism_trial_id</t>
   </si>
   <si>
-    <t>Mount Sinai</t>
-  </si>
-  <si>
-    <t>Express Somatic Human WES (Deep Coverage) v1.1</t>
-  </si>
-  <si>
-    <t>Hyper Prep ICE Exome Express: 1.0</t>
-  </si>
-  <si>
-    <t>Illumina - NextSeq 550</t>
-  </si>
-  <si>
-    <t>Paired</t>
-  </si>
-  <si>
-    <t>whole_exome_illumina_coding_v1</t>
-  </si>
-  <si>
     <t>CTTTPP111.00</t>
   </si>
   <si>
+    <t>/local/path/to/fwd.1.1.1.fastq</t>
+  </si>
+  <si>
+    <t>/local/path/to/rev.1.1.1.fastq</t>
+  </si>
+  <si>
     <t>CTTTPP121.00</t>
   </si>
   <si>
-    <t>/local/path/to/fwd.1.1.1.fastq</t>
-  </si>
-  <si>
-    <t>/local/path/to/rev.1.1.1.fastq</t>
-  </si>
-  <si>
     <t>/local/path/to/fwd.1.2.1.fastq</t>
   </si>
   <si>
     <t>/local/path/to/rev.1.2.1.fastq</t>
-  </si>
-  <si>
-    <t>test_prism_trial_id_run_1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -342,14 +455,8 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -371,6 +478,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5FA3F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -413,18 +526,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -765,8 +884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -775,170 +894,170 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-    </row>
-    <row r="2" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="C3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="C4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="C5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="C6" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="C7" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="C8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="2">
         <v>100</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="C10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="3" t="s">
         <v>19</v>
       </c>
     </row>
@@ -947,15 +1066,15 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" s="3">
+        <v>67</v>
+      </c>
+      <c r="E14" s="6">
         <v>40179</v>
       </c>
       <c r="F14">
@@ -967,15 +1086,15 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="D15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="3">
+        <v>70</v>
+      </c>
+      <c r="E15" s="6">
         <v>40179</v>
       </c>
       <c r="F15">
@@ -1978,22 +2097,22 @@
     <mergeCell ref="B12:F12"/>
   </mergeCells>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{35009C75-D215-2840-9826-04533ED6BD99}">
       <formula1>"DFCI,Mount Sinai,Stanford,MD Anderson"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{ED481183-8BAB-8045-B2B2-4A17594E488B}">
       <formula1>"Express Somatic Human WES (Deep Coverage) v1.1"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6" xr:uid="{6A02D14E-26AF-8B4C-9294-FF123682E275}">
       <formula1>"Hyper Prep ICE Exome Express: 1.0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7" xr:uid="{FCFF2FD4-DBD0-7047-8716-4078CC1D48C7}">
       <formula1>"Illumina - HiSeq 2500,Illumina - HiSeq 3000,Illumina - NextSeq 550,Illumina - HiSeq 4000,Illumina - NovaSeq 6000"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8" xr:uid="{CD02A45E-A421-F04E-85CA-672B69BC9A23}">
       <formula1>"Paired,Single"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{8557FF76-A65E-4A42-A68D-4C2DA3CCF04D}">
       <formula1>"whole_exome_illumina_coding_v1"</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="E14:E213" xr:uid="{00000000-0002-0000-0000-000006000000}">
@@ -2003,4 +2122,300 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B1:E17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="101" width="30.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B1" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="B1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="101" width="30.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed tests for dropped assay_run_id in wes
</commit_message>
<xml_diff>
--- a/template_examples/wes_template.xlsx
+++ b/template_examples/wes_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2003E7DD-E808-D14B-ACE1-0217443741E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C078348-3D15-904C-9BB7-6470CFE2A78E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7880" yWindow="5000" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,20 +27,7 @@
     <author>CIDC</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>User defined unique identifier for this assay run.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -53,7 +40,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -66,7 +53,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -79,7 +66,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -92,7 +79,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -105,7 +92,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -118,7 +105,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -131,7 +118,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -144,7 +131,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -157,7 +144,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
+    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -170,7 +157,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
+    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -183,7 +170,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
+    <comment ref="E12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -196,7 +183,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
+    <comment ref="F12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -214,7 +201,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="70">
   <si>
     <t>#t</t>
   </si>
@@ -403,9 +390,6 @@
   </si>
   <si>
     <t>whole_exome_illumina_coding_v1</t>
-  </si>
-  <si>
-    <t>test_prism_trial_id_run_1</t>
   </si>
   <si>
     <t>test_prism_trial_id</t>
@@ -540,10 +524,10 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -882,10 +866,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F213"/>
+  <dimension ref="A1:F212"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="B2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -898,20 +882,20 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
     </row>
     <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>63</v>
@@ -925,38 +909,38 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -967,10 +951,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -981,10 +965,10 @@
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -995,10 +979,10 @@
         <v>2</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>60</v>
+        <v>10</v>
+      </c>
+      <c r="C8" s="2">
+        <v>100</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -1009,56 +993,62 @@
         <v>2</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="2">
-        <v>100</v>
+        <v>11</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B12" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>19</v>
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="5">
+        <v>40179</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1066,15 +1056,15 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C14" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E14" s="6">
+        <v>69</v>
+      </c>
+      <c r="E14" s="5">
         <v>40179</v>
       </c>
       <c r="F14">
@@ -1085,21 +1075,6 @@
       <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>68</v>
-      </c>
-      <c r="C15" t="s">
-        <v>69</v>
-      </c>
-      <c r="D15" t="s">
-        <v>70</v>
-      </c>
-      <c r="E15" s="6">
-        <v>40179</v>
-      </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -2083,40 +2058,35 @@
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A213" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B11:F11"/>
   </mergeCells>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{35009C75-D215-2840-9826-04533ED6BD99}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{35009C75-D215-2840-9826-04533ED6BD99}">
       <formula1>"DFCI,Mount Sinai,Stanford,MD Anderson"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{ED481183-8BAB-8045-B2B2-4A17594E488B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{ED481183-8BAB-8045-B2B2-4A17594E488B}">
       <formula1>"Express Somatic Human WES (Deep Coverage) v1.1"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6" xr:uid="{6A02D14E-26AF-8B4C-9294-FF123682E275}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{6A02D14E-26AF-8B4C-9294-FF123682E275}">
       <formula1>"Hyper Prep ICE Exome Express: 1.0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7" xr:uid="{FCFF2FD4-DBD0-7047-8716-4078CC1D48C7}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6" xr:uid="{FCFF2FD4-DBD0-7047-8716-4078CC1D48C7}">
       <formula1>"Illumina - HiSeq 2500,Illumina - HiSeq 3000,Illumina - NextSeq 550,Illumina - HiSeq 4000,Illumina - NovaSeq 6000"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8" xr:uid="{CD02A45E-A421-F04E-85CA-672B69BC9A23}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7" xr:uid="{CD02A45E-A421-F04E-85CA-672B69BC9A23}">
       <formula1>"Paired,Single"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{8557FF76-A65E-4A42-A68D-4C2DA3CCF04D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{8557FF76-A65E-4A42-A68D-4C2DA3CCF04D}">
       <formula1>"whole_exome_illumina_coding_v1"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="E14:E213" xr:uid="{00000000-0002-0000-0000-000006000000}">
-      <formula1>AND(ISNUMBER(E14:E213),LEFT(CELL("format",E14:E213),1)="D")</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="E13:E212" xr:uid="{00000000-0002-0000-0000-000006000000}">
+      <formula1>AND(ISNUMBER(E13:E212),LEFT(CELL("format",E13:E212),1)="D")</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
wes template fastq.gz support
</commit_message>
<xml_diff>
--- a/template_examples/wes_template.xlsx
+++ b/template_examples/wes_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C078348-3D15-904C-9BB7-6470CFE2A78E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D062EF8-EFD7-A546-8136-1EEA9D316E3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7880" yWindow="5000" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -398,19 +398,19 @@
     <t>CTTTPP111.00</t>
   </si>
   <si>
-    <t>/local/path/to/fwd.1.1.1.fastq</t>
-  </si>
-  <si>
-    <t>/local/path/to/rev.1.1.1.fastq</t>
-  </si>
-  <si>
     <t>CTTTPP121.00</t>
   </si>
   <si>
-    <t>/local/path/to/fwd.1.2.1.fastq</t>
-  </si>
-  <si>
-    <t>/local/path/to/rev.1.2.1.fastq</t>
+    <t>/local/path/to/fwd.1.1.1.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/fwd.1.2.1.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/rev.1.1.1.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/rev.1.2.1.fastq.gz</t>
   </si>
 </sst>
 </file>
@@ -868,8 +868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1039,10 +1039,10 @@
         <v>64</v>
       </c>
       <c r="C13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D13" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E13" s="5">
         <v>40179</v>
@@ -1056,10 +1056,10 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" t="s">
         <v>67</v>
-      </c>
-      <c r="C14" t="s">
-        <v>68</v>
       </c>
       <c r="D14" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
inputs changed from fastqs to bam
</commit_message>
<xml_diff>
--- a/template_examples/wes_template.xlsx
+++ b/template_examples/wes_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D062EF8-EFD7-A546-8136-1EEA9D316E3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6108A749-346C-7049-9C89-91B7BE9B38F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7880" yWindow="5000" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2700" yWindow="6120" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WES" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
     <author>CIDC</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -40,7 +40,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -53,7 +53,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -66,7 +66,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -79,7 +79,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -92,7 +92,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -105,7 +105,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -118,7 +118,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -131,7 +131,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -144,7 +144,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
+    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -157,20 +157,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Path to a file on a user's computer.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
+    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -183,7 +170,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
+    <comment ref="E12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -201,7 +188,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="65">
   <si>
     <t>#t</t>
   </si>
@@ -212,9 +199,6 @@
     <t>#p</t>
   </si>
   <si>
-    <t>Assay run id</t>
-  </si>
-  <si>
     <t>Protocol identifier</t>
   </si>
   <si>
@@ -251,10 +235,7 @@
     <t>Cimac id</t>
   </si>
   <si>
-    <t>Forward fastq</t>
-  </si>
-  <si>
-    <t>Reverse fastq</t>
+    <t>Bam</t>
   </si>
   <si>
     <t>Sequencing date</t>
@@ -272,9 +253,6 @@
     <t>String</t>
   </si>
   <si>
-    <t>User defined unique identifier for this assay run.</t>
-  </si>
-  <si>
     <t>Trial identifier used by lead organization, ie. Center for Experimental Therapeutics Program (CTEP) ID or Industry Sponsored ID.  This is usually a short identifier. Example: E4412.</t>
   </si>
   <si>
@@ -401,23 +379,17 @@
     <t>CTTTPP121.00</t>
   </si>
   <si>
-    <t>/local/path/to/fwd.1.1.1.fastq.gz</t>
-  </si>
-  <si>
-    <t>/local/path/to/fwd.1.2.1.fastq.gz</t>
-  </si>
-  <si>
-    <t>/local/path/to/rev.1.1.1.fastq.gz</t>
-  </si>
-  <si>
-    <t>/local/path/to/rev.1.2.1.fastq.gz</t>
+    <t>/local/path/to/data.1.bam</t>
+  </si>
+  <si>
+    <t>/local/path/to/data.2.bam</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -438,6 +410,13 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -510,7 +489,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -524,10 +503,11 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -866,10 +846,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F212"/>
+  <dimension ref="A1:E212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -878,1215 +858,1196 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-    </row>
-    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+    </row>
+    <row r="2" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:5" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="2">
         <v>100</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B11" s="6" t="s">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
       <c r="B12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="7">
+        <v>40179</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C13" t="s">
-        <v>66</v>
-      </c>
-      <c r="D13" t="s">
-        <v>68</v>
-      </c>
-      <c r="E13" s="5">
+      <c r="D14" s="7">
         <v>40179</v>
       </c>
-      <c r="F13">
+      <c r="E14">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" t="s">
-        <v>65</v>
-      </c>
-      <c r="C14" t="s">
-        <v>67</v>
-      </c>
-      <c r="D14" t="s">
-        <v>69</v>
-      </c>
-      <c r="E14" s="5">
-        <v>40179</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B11:E11"/>
   </mergeCells>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{35009C75-D215-2840-9826-04533ED6BD99}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{88D52335-C10A-584D-B6CE-499F4159B4F6}">
       <formula1>"DFCI,Mount Sinai,Stanford,MD Anderson"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{ED481183-8BAB-8045-B2B2-4A17594E488B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{33100B37-E141-F242-955F-8BF04C8410C1}">
       <formula1>"Express Somatic Human WES (Deep Coverage) v1.1"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{6A02D14E-26AF-8B4C-9294-FF123682E275}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{91650D31-007E-BB47-9AF5-4FE6765A8632}">
       <formula1>"Hyper Prep ICE Exome Express: 1.0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6" xr:uid="{FCFF2FD4-DBD0-7047-8716-4078CC1D48C7}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6" xr:uid="{64EA2867-8E88-A648-8DE5-C18F99EFB01B}">
       <formula1>"Illumina - HiSeq 2500,Illumina - HiSeq 3000,Illumina - NextSeq 550,Illumina - HiSeq 4000,Illumina - NovaSeq 6000"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7" xr:uid="{CD02A45E-A421-F04E-85CA-672B69BC9A23}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7" xr:uid="{1DA8C959-F2FB-134B-BD75-175D3F24E927}">
       <formula1>"Paired,Single"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{8557FF76-A65E-4A42-A68D-4C2DA3CCF04D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{6B9F82CD-5460-3047-B6FF-E402638A08EF}">
       <formula1>"whole_exome_illumina_coding_v1"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="E13:E212" xr:uid="{00000000-0002-0000-0000-000006000000}">
-      <formula1>AND(ISNUMBER(E13:E212),LEFT(CELL("format",E13:E212),1)="D")</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="D13:D212" xr:uid="{00000000-0002-0000-0000-000006000000}">
+      <formula1>AND(ISNUMBER(D13:D212),LEFT(CELL("format",D13:D212),1)="D")</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2096,7 +2057,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B1:E17"/>
+  <dimension ref="B1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2107,12 +2068,12 @@
   <sheetData>
     <row r="1" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B1" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2120,10 +2081,10 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2134,6 +2095,9 @@
         <v>22</v>
       </c>
       <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2142,13 +2106,13 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
         <v>25</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>26</v>
-      </c>
-      <c r="E5" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2156,13 +2120,13 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" t="s">
         <v>28</v>
-      </c>
-      <c r="E6" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2170,13 +2134,13 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
         <v>30</v>
-      </c>
-      <c r="E7" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2184,13 +2148,13 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s">
         <v>32</v>
-      </c>
-      <c r="E8" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2198,13 +2162,10 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s">
         <v>34</v>
-      </c>
-      <c r="E9" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2212,28 +2173,31 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" t="s">
         <v>36</v>
       </c>
-      <c r="D10" t="s">
+    </row>
+    <row r="11" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="B11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" t="s">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
         <v>38</v>
       </c>
-      <c r="E11" t="s">
+      <c r="D12" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="12" spans="2:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s">
+      <c r="E12" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2242,13 +2206,10 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
         <v>41</v>
-      </c>
-      <c r="D13" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
@@ -2256,10 +2217,10 @@
         <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="D14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">
@@ -2267,32 +2228,10 @@
         <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="D15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B16" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" t="s">
         <v>45</v>
-      </c>
-      <c r="D16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B17" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -2314,74 +2253,74 @@
   <sheetData>
     <row r="1" spans="2:7" ht="16" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="G1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "inputs changed from fastqs to bam"
This reverts commit cd911087516cd5fc13445dfbbc4843a452c3eb3e.
</commit_message>
<xml_diff>
--- a/template_examples/wes_template.xlsx
+++ b/template_examples/wes_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6108A749-346C-7049-9C89-91B7BE9B38F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D062EF8-EFD7-A546-8136-1EEA9D316E3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2700" yWindow="6120" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7880" yWindow="5000" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WES" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
     <author>CIDC</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -40,7 +40,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -53,7 +53,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -66,7 +66,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -79,7 +79,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -92,7 +92,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -105,7 +105,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -118,7 +118,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -131,7 +131,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -144,7 +144,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -157,7 +157,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
+    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Path to a file on a user's computer.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -170,7 +183,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
+    <comment ref="F12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -188,7 +201,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="70">
   <si>
     <t>#t</t>
   </si>
@@ -199,6 +212,9 @@
     <t>#p</t>
   </si>
   <si>
+    <t>Assay run id</t>
+  </si>
+  <si>
     <t>Protocol identifier</t>
   </si>
   <si>
@@ -235,7 +251,10 @@
     <t>Cimac id</t>
   </si>
   <si>
-    <t>Bam</t>
+    <t>Forward fastq</t>
+  </si>
+  <si>
+    <t>Reverse fastq</t>
   </si>
   <si>
     <t>Sequencing date</t>
@@ -253,6 +272,9 @@
     <t>String</t>
   </si>
   <si>
+    <t>User defined unique identifier for this assay run.</t>
+  </si>
+  <si>
     <t>Trial identifier used by lead organization, ie. Center for Experimental Therapeutics Program (CTEP) ID or Industry Sponsored ID.  This is usually a short identifier. Example: E4412.</t>
   </si>
   <si>
@@ -379,17 +401,23 @@
     <t>CTTTPP121.00</t>
   </si>
   <si>
-    <t>/local/path/to/data.1.bam</t>
-  </si>
-  <si>
-    <t>/local/path/to/data.2.bam</t>
+    <t>/local/path/to/fwd.1.1.1.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/fwd.1.2.1.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/rev.1.1.1.fastq.gz</t>
+  </si>
+  <si>
+    <t>/local/path/to/rev.1.2.1.fastq.gz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -410,13 +438,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -489,7 +510,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -503,11 +524,10 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -846,10 +866,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E212"/>
+  <dimension ref="A1:F212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13:E14"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -858,1196 +878,1215 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-    </row>
-    <row r="2" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C8" s="2">
         <v>100</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C13" t="s">
-        <v>63</v>
-      </c>
-      <c r="D13" s="7">
+        <v>66</v>
+      </c>
+      <c r="D13" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="5">
         <v>40179</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="D14" s="7">
+        <v>65</v>
+      </c>
+      <c r="C14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" s="5">
         <v>40179</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B11:F11"/>
   </mergeCells>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{88D52335-C10A-584D-B6CE-499F4159B4F6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{35009C75-D215-2840-9826-04533ED6BD99}">
       <formula1>"DFCI,Mount Sinai,Stanford,MD Anderson"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{33100B37-E141-F242-955F-8BF04C8410C1}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{ED481183-8BAB-8045-B2B2-4A17594E488B}">
       <formula1>"Express Somatic Human WES (Deep Coverage) v1.1"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{91650D31-007E-BB47-9AF5-4FE6765A8632}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{6A02D14E-26AF-8B4C-9294-FF123682E275}">
       <formula1>"Hyper Prep ICE Exome Express: 1.0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6" xr:uid="{64EA2867-8E88-A648-8DE5-C18F99EFB01B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6" xr:uid="{FCFF2FD4-DBD0-7047-8716-4078CC1D48C7}">
       <formula1>"Illumina - HiSeq 2500,Illumina - HiSeq 3000,Illumina - NextSeq 550,Illumina - HiSeq 4000,Illumina - NovaSeq 6000"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7" xr:uid="{1DA8C959-F2FB-134B-BD75-175D3F24E927}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7" xr:uid="{CD02A45E-A421-F04E-85CA-672B69BC9A23}">
       <formula1>"Paired,Single"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{6B9F82CD-5460-3047-B6FF-E402638A08EF}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{8557FF76-A65E-4A42-A68D-4C2DA3CCF04D}">
       <formula1>"whole_exome_illumina_coding_v1"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="D13:D212" xr:uid="{00000000-0002-0000-0000-000006000000}">
-      <formula1>AND(ISNUMBER(D13:D212),LEFT(CELL("format",D13:D212),1)="D")</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="E13:E212" xr:uid="{00000000-0002-0000-0000-000006000000}">
+      <formula1>AND(ISNUMBER(E13:E212),LEFT(CELL("format",E13:E212),1)="D")</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2057,7 +2096,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B1:E15"/>
+  <dimension ref="B1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2068,12 +2107,12 @@
   <sheetData>
     <row r="1" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B1" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2081,10 +2120,10 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2095,9 +2134,6 @@
         <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2106,13 +2142,13 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2120,13 +2156,13 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2134,13 +2170,13 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2148,13 +2184,13 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2162,10 +2198,13 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
         <v>34</v>
+      </c>
+      <c r="E9" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2173,31 +2212,28 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="B11" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
         <v>38</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E11" t="s">
         <v>39</v>
       </c>
-      <c r="E12" t="s">
+    </row>
+    <row r="12" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2206,10 +2242,13 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="D13" t="s">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="E13" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
@@ -2217,10 +2256,10 @@
         <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="D14" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">
@@ -2228,10 +2267,32 @@
         <v>17</v>
       </c>
       <c r="C15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" t="s">
         <v>44</v>
       </c>
-      <c r="D15" t="s">
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" t="s">
         <v>45</v>
+      </c>
+      <c r="D16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -2253,74 +2314,74 @@
   <sheetData>
     <row r="1" spans="2:7" ht="16" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="F2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="G2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="F3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E6" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>